<commit_message>
comentado el agregar imagen en el formulario de humedal para que no aparezca
</commit_message>
<xml_diff>
--- a/Cambios y Pruebas Hechas.xlsx
+++ b/Cambios y Pruebas Hechas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
   <si>
     <t>Cambios</t>
   </si>
@@ -92,6 +92,27 @@
   </si>
   <si>
     <t>Carga de cuenca</t>
+  </si>
+  <si>
+    <t>Mi Rama</t>
+  </si>
+  <si>
+    <t>Mensaje de adbertencia campo obligatorio incompleto (Cuenca)</t>
+  </si>
+  <si>
+    <t>Mensaje de adbertencia campo obligatorio incompleto (Complejo)</t>
+  </si>
+  <si>
+    <t>Mensaje de adbertencia campo obligatorio incompleto (Persona)</t>
+  </si>
+  <si>
+    <t>Mensaje de adbertencia campo obligatorio incompleto (Presiones)</t>
+  </si>
+  <si>
+    <t>Mensaje de adbertencia campo obligatorio incompleto (Fauna)</t>
+  </si>
+  <si>
+    <t>Mensaje de adbertencia campo obligatorio incompleto (Flora)</t>
   </si>
 </sst>
 </file>
@@ -152,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -246,26 +267,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -292,10 +298,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -601,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +632,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -647,7 +661,7 @@
       <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -664,7 +678,7 @@
       <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -681,7 +695,7 @@
       <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -698,7 +712,7 @@
       <c r="E5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -715,7 +729,7 @@
       <c r="E6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="15" t="s">
         <v>24</v>
       </c>
       <c r="I6" s="8"/>
@@ -733,7 +747,7 @@
       <c r="E7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -750,7 +764,7 @@
       <c r="E8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -767,7 +781,7 @@
       <c r="E9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -781,7 +795,7 @@
       <c r="E10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="4"/>
@@ -796,7 +810,7 @@
       <c r="E11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="4"/>
@@ -812,7 +826,7 @@
       <c r="E12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -823,17 +837,127 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="12"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="14"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+    <row r="14" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="17"/>
+      <c r="D21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="17"/>
+      <c r="D22" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="18"/>
+      <c r="D23" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="17"/>
+      <c r="D24" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="17"/>
+      <c r="D25" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>